<commit_message>
Arreglo tabla de Cliente
Se le agregan los datos de la tabla cliente
</commit_message>
<xml_diff>
--- a/tablas.xlsx
+++ b/tablas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\OneDrive\Documentos\ASP.NET\prueba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prueba\prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47436E54-01FA-48FE-B67A-62C0658A9E0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B6643F-BE41-4E69-8CCB-1051C64F9D10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{375CCFBA-C5CB-4C66-B980-6EC719382F9C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Tabla de Usuario</t>
   </si>
@@ -163,13 +163,34 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Nombre_contacto</t>
+  </si>
+  <si>
+    <t>correoele_contacto</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Angela Salazar</t>
+  </si>
+  <si>
+    <t>angela@bncr.fi.cr</t>
+  </si>
+  <si>
+    <t>Jefa directa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +202,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -223,11 +252,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,8 +317,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -296,15 +344,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -319,8 +367,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2571750" y="5076825"/>
-          <a:ext cx="4895850" cy="1247775"/>
+          <a:off x="3067050" y="6905625"/>
+          <a:ext cx="5095875" cy="1247775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -669,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB104980-8D69-487B-952D-A40CEBF0CC0C}">
   <dimension ref="A2:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +726,7 @@
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="23.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.140625" customWidth="1"/>
     <col min="11" max="11" width="21.140625" customWidth="1"/>
@@ -964,7 +1013,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>7</v>
       </c>
@@ -981,7 +1030,7 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K19" s="3" t="s">
         <v>36</v>
       </c>
@@ -990,12 +1039,24 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>9</v>
@@ -1013,14 +1074,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="C21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2222222</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="H21" s="2">
         <v>1</v>
       </c>
@@ -1037,10 +1109,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="1"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
       <c r="H22" s="2">
         <v>2</v>
       </c>
@@ -1057,9 +1132,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1075,8 +1154,11 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D21" r:id="rId1" xr:uid="{DCA0779F-5A42-450F-B65C-2D4C4A7E9A16}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio a las tablas
Varios cambios a las tablas
</commit_message>
<xml_diff>
--- a/tablas.xlsx
+++ b/tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prueba\prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B6643F-BE41-4E69-8CCB-1051C64F9D10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72C157B-855F-4245-98DA-E418BF873A53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{375CCFBA-C5CB-4C66-B980-6EC719382F9C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Tabla de Usuario</t>
   </si>
@@ -39,12 +39,6 @@
     <t>id_usuario</t>
   </si>
   <si>
-    <t>apellido1</t>
-  </si>
-  <si>
-    <t>apellido2</t>
-  </si>
-  <si>
     <t>nickname</t>
   </si>
   <si>
@@ -75,18 +69,9 @@
     <t>id_dcreado</t>
   </si>
   <si>
-    <t>Titulo_dcreado</t>
-  </si>
-  <si>
-    <t>detalle_dcreado</t>
-  </si>
-  <si>
     <t>detalalle_proyecto</t>
   </si>
   <si>
-    <t>consecutivo_dcreado</t>
-  </si>
-  <si>
     <t>consecutivo_costo</t>
   </si>
   <si>
@@ -99,30 +84,12 @@
     <t>tabla documento subido</t>
   </si>
   <si>
-    <t>Titulo_dsubido</t>
-  </si>
-  <si>
-    <t>detalle_dsubido</t>
-  </si>
-  <si>
-    <t>consecutivo_dsubido</t>
-  </si>
-  <si>
     <t>pk</t>
   </si>
   <si>
-    <t>id_dsubido</t>
-  </si>
-  <si>
     <t>andreina</t>
   </si>
   <si>
-    <t>porras</t>
-  </si>
-  <si>
-    <t>castro</t>
-  </si>
-  <si>
     <t>aporras</t>
   </si>
   <si>
@@ -135,9 +102,6 @@
     <t>edificio5</t>
   </si>
   <si>
-    <t>id proyecto</t>
-  </si>
-  <si>
     <t>licitacion calle 27</t>
   </si>
   <si>
@@ -156,9 +120,6 @@
     <t>titulos del profesional</t>
   </si>
   <si>
-    <t>id_dtotal</t>
-  </si>
-  <si>
     <t>paja</t>
   </si>
   <si>
@@ -184,13 +145,139 @@
   </si>
   <si>
     <t>Jefa directa</t>
+  </si>
+  <si>
+    <t>apellidos</t>
+  </si>
+  <si>
+    <t>porras castro</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>aporras@</t>
+  </si>
+  <si>
+    <t>Clave</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>** esta tabla de centro de costos creo que no es necesaria porque el consecutivo se le da al proyecto y no conlleva mas informacion se coloca un</t>
+  </si>
+  <si>
+    <t>incremental solo por debajo ya que el usuario no debe manipularlo</t>
+  </si>
+  <si>
+    <t>Centro_costos</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Nombre_proyecto</t>
+  </si>
+  <si>
+    <t>Autogenerado</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Barranca</t>
+  </si>
+  <si>
+    <t>Nombre_Creado</t>
+  </si>
+  <si>
+    <t>Asunto_creado</t>
+  </si>
+  <si>
+    <t>Descripcion_creado</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>kkkkkkkk</t>
+  </si>
+  <si>
+    <t>kkkkkkkkkk</t>
+  </si>
+  <si>
+    <t>total documentos creados por Proyecto</t>
+  </si>
+  <si>
+    <t>id_total_docu</t>
+  </si>
+  <si>
+    <t>proyecto</t>
+  </si>
+  <si>
+    <t>Consecutivo</t>
+  </si>
+  <si>
+    <t>*revisar el tema de la numeracion de los consecutivos por proyecto</t>
+  </si>
+  <si>
+    <t>Consecutivo_docu</t>
+  </si>
+  <si>
+    <t>Consecutivo_total</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>id_subido</t>
+  </si>
+  <si>
+    <t>Varbynary</t>
+  </si>
+  <si>
+    <t>Documento</t>
+  </si>
+  <si>
+    <t>Varbinary</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>2019-01-01-01</t>
+  </si>
+  <si>
+    <t>2019-01-02-02</t>
+  </si>
+  <si>
+    <t>2019-02-01-03</t>
+  </si>
+  <si>
+    <t>2019-03-01-04</t>
+  </si>
+  <si>
+    <t>Total_subid</t>
+  </si>
+  <si>
+    <t>Tomada de toda la info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +301,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -229,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -265,12 +367,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -284,8 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,18 +406,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,8 +424,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -343,16 +485,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -367,7 +509,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3067050" y="6905625"/>
+          <a:off x="7096125" y="8763000"/>
           <a:ext cx="5095875" cy="1247775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -715,44 +857,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB104980-8D69-487B-952D-A40CEBF0CC0C}">
-  <dimension ref="A2:O23"/>
+  <dimension ref="A2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" style="3" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="3"/>
+    <col min="14" max="14" width="13" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="J2" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="6"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -760,24 +899,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="J4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>18</v>
+      <c r="F4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -785,26 +922,24 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1234</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -812,15 +947,9 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <v>2</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -828,250 +957,235 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="I9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="B9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="L10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
+      <c r="A11" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>34</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
-      <c r="M12" s="8">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2">
+        <v>28</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
         <v>2</v>
       </c>
-      <c r="E13" s="16">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="H13" s="4">
         <v>2</v>
       </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="5"/>
+      <c r="I13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2">
+        <v>29</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
         <v>3</v>
       </c>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="I14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="12"/>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>4</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="B18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="F18" s="12"/>
+      <c r="I18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" s="5"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1079,86 +1193,299 @@
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2">
         <v>2222222</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="9">
-        <v>2315454564564</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
-      <c r="L21" s="2">
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="5"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="H22" s="2">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="3">
         <v>2</v>
       </c>
-      <c r="I22" s="2">
-        <v>3666366</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
-      <c r="L22" s="2">
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="H23" s="3">
+        <v>3</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="23"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="26">
+        <v>1</v>
+      </c>
+      <c r="B28" s="26">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="26">
+        <v>2</v>
+      </c>
+      <c r="B29" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>1</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D40" s="1"/>
+      <c r="F40" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="7">
+        <v>2315454564564</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>2</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="19">
+        <v>3666366</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="6">
+        <v>2019</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="H18:L18"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A39:G39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{DCA0779F-5A42-450F-B65C-2D4C4A7E9A16}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{A900865D-4E0E-4897-958A-F269939223D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>